<commit_message>
Adding Data Driven Test Runner , Extent Report ,Screenshot and test data for signin
</commit_message>
<xml_diff>
--- a/TestData/DSAlgo.xlsx
+++ b/TestData/DSAlgo.xlsx
@@ -1,14 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33C7ABAF-4D10-4D5E-9C9B-A9FDE690A2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shiva\NumpyNinja\SDET229-DSAlgo\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1758AE-A483-41D2-A542-0DB744675820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TreeLinksAndTitles" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -26,12 +32,15 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>topicLinks</t>
   </si>
@@ -73,13 +82,61 @@
   </si>
   <si>
     <t>Implementation Of BST</t>
+  </si>
+  <si>
+    <t>SignInScenario</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Verify valid Login Credentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test-229 </t>
+  </si>
+  <si>
+    <t>Shivagami229.</t>
+  </si>
+  <si>
+    <t>You are logged in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wel123Fine </t>
+  </si>
+  <si>
+    <t>Verify invalid Login Credentials</t>
+  </si>
+  <si>
+    <t>Test-229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid Username and Password </t>
+  </si>
+  <si>
+    <t>Test-228</t>
+  </si>
+  <si>
+    <t>Test$229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shivagami229. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +149,12 @@
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,10 +177,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -456,17 +524,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="70" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" customWidth="1"/>
+    <col min="2" max="2" width="48.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75">
+    <row r="1" spans="1:2" ht="18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -474,7 +542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75">
+    <row r="2" spans="1:2" ht="18">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -482,7 +550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75">
+    <row r="3" spans="1:2" ht="18">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -490,7 +558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75">
+    <row r="4" spans="1:2" ht="18">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -498,7 +566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75">
+    <row r="5" spans="1:2" ht="18">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -506,7 +574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75">
+    <row r="6" spans="1:2" ht="18">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -514,7 +582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75">
+    <row r="7" spans="1:2" ht="18">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -522,7 +590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="37.5">
+    <row r="8" spans="1:2" ht="18">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -530,7 +598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18.75">
+    <row r="9" spans="1:2" ht="18">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -538,7 +606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18.75">
+    <row r="10" spans="1:2" ht="18">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -546,7 +614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18.75">
+    <row r="11" spans="1:2" ht="18">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -554,7 +622,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.75">
+    <row r="12" spans="1:2" ht="18">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -562,12 +630,111 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18.75">
+    <row r="13" spans="1:2" ht="18">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87098745-8CC1-4807-8F99-5F42923EBD4B}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="3">
+        <v>123456789</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>